<commit_message>
Completed 27,28 and 20. Completed coding all 28 test cases
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/WorkbookUploadTemplates/WorkbookItemsTemplate-PN.xlsx
+++ b/resources/ExcelsheetData/WorkbookUploadTemplates/WorkbookItemsTemplate-PN.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="9">
   <si>
     <t>PART_NUMBER</t>
   </si>
@@ -32,6 +32,15 @@
   </si>
   <si>
     <t>AutomationTestPN 2</t>
+  </si>
+  <si>
+    <t>Auto TestPN 1</t>
+  </si>
+  <si>
+    <t>Auto TestPN 2</t>
+  </si>
+  <si>
+    <t>Auto TestPN 3</t>
   </si>
 </sst>
 </file>
@@ -393,17 +402,17 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>